<commit_message>
wyjebane 2 puste kolumny z excela
</commit_message>
<xml_diff>
--- a/sklep_2.xlsx
+++ b/sklep_2.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piter\Desktop\DOBRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aghedupl-my.sharepoint.com/personal/nalepkap_student_agh_edu_pl/Documents/Sem5/SVD/KERFUS_V2137/SWD_Kerfus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB9D908-C486-4DD6-8647-2A8F3F71BC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0DB9D908-C486-4DD6-8647-2A8F3F71BC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9DA3F1-D65D-4178-A6FB-3EDC28C686D9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{983B0401-862A-4A11-94D6-A974676171F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{983B0401-862A-4A11-94D6-A974676171F9}"/>
   </bookViews>
   <sheets>
     <sheet name="mapa" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Legenda</t>
   </si>
@@ -78,20 +78,14 @@
     <t>odleglosc od półki</t>
   </si>
   <si>
-    <t>odleglosc od bazy</t>
-  </si>
-  <si>
     <t>wsp. popularnosci</t>
-  </si>
-  <si>
-    <t>odleglosc punktu od aktulanej pozycji robota</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,14 +190,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -316,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -334,14 +320,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -728,186 +712,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC73091E-0747-4333-9BE2-227938726090}">
   <dimension ref="A1:BJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="60" max="60" width="38.21875" customWidth="1"/>
-    <col min="61" max="61" width="7.33203125" customWidth="1"/>
-    <col min="62" max="62" width="45.33203125" customWidth="1"/>
+    <col min="60" max="60" width="38.28515625" customWidth="1"/>
+    <col min="61" max="61" width="7.28515625" customWidth="1"/>
+    <col min="62" max="62" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="21">
-        <v>0</v>
-      </c>
-      <c r="C1" s="22">
-        <v>1</v>
-      </c>
-      <c r="D1" s="21">
+    <row r="1" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="19">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19">
         <v>2</v>
       </c>
-      <c r="E1" s="22">
+      <c r="E1" s="20">
         <v>3</v>
       </c>
-      <c r="F1" s="21">
+      <c r="F1" s="19">
         <v>4</v>
       </c>
-      <c r="G1" s="22">
+      <c r="G1" s="20">
         <v>5</v>
       </c>
-      <c r="H1" s="21">
+      <c r="H1" s="19">
         <v>6</v>
       </c>
-      <c r="I1" s="22">
+      <c r="I1" s="20">
         <v>7</v>
       </c>
-      <c r="J1" s="21">
+      <c r="J1" s="19">
         <v>8</v>
       </c>
-      <c r="K1" s="22">
+      <c r="K1" s="20">
         <v>9</v>
       </c>
-      <c r="L1" s="21">
+      <c r="L1" s="19">
         <v>10</v>
       </c>
-      <c r="M1" s="22">
+      <c r="M1" s="20">
         <v>11</v>
       </c>
-      <c r="N1" s="21">
+      <c r="N1" s="19">
         <v>12</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="20">
         <v>13</v>
       </c>
-      <c r="P1" s="21">
+      <c r="P1" s="19">
         <v>14</v>
       </c>
-      <c r="Q1" s="22">
+      <c r="Q1" s="20">
         <v>15</v>
       </c>
-      <c r="R1" s="21">
+      <c r="R1" s="19">
         <v>16</v>
       </c>
-      <c r="S1" s="22">
+      <c r="S1" s="20">
         <v>17</v>
       </c>
-      <c r="T1" s="21">
+      <c r="T1" s="19">
         <v>18</v>
       </c>
-      <c r="U1" s="22">
+      <c r="U1" s="20">
         <v>19</v>
       </c>
-      <c r="V1" s="21">
+      <c r="V1" s="19">
         <v>20</v>
       </c>
-      <c r="W1" s="22">
+      <c r="W1" s="20">
         <v>21</v>
       </c>
-      <c r="X1" s="21">
+      <c r="X1" s="19">
         <v>22</v>
       </c>
-      <c r="Y1" s="22">
+      <c r="Y1" s="20">
         <v>23</v>
       </c>
-      <c r="Z1" s="21">
+      <c r="Z1" s="19">
         <v>24</v>
       </c>
-      <c r="AA1" s="22">
+      <c r="AA1" s="20">
         <v>25</v>
       </c>
-      <c r="AB1" s="21">
+      <c r="AB1" s="19">
         <v>26</v>
       </c>
-      <c r="AC1" s="22">
+      <c r="AC1" s="20">
         <v>27</v>
       </c>
-      <c r="AD1" s="21">
+      <c r="AD1" s="19">
         <v>28</v>
       </c>
-      <c r="AE1" s="22">
+      <c r="AE1" s="20">
         <v>29</v>
       </c>
-      <c r="AF1" s="21">
+      <c r="AF1" s="19">
         <v>30</v>
       </c>
-      <c r="AG1" s="22">
+      <c r="AG1" s="20">
         <v>31</v>
       </c>
-      <c r="AH1" s="21">
+      <c r="AH1" s="19">
         <v>32</v>
       </c>
-      <c r="AI1" s="22">
+      <c r="AI1" s="20">
         <v>33</v>
       </c>
-      <c r="AJ1" s="21">
+      <c r="AJ1" s="19">
         <v>34</v>
       </c>
-      <c r="AK1" s="22">
+      <c r="AK1" s="20">
         <v>35</v>
       </c>
-      <c r="AL1" s="21">
+      <c r="AL1" s="19">
         <v>36</v>
       </c>
-      <c r="AM1" s="22">
+      <c r="AM1" s="20">
         <v>37</v>
       </c>
-      <c r="AN1" s="21">
+      <c r="AN1" s="19">
         <v>38</v>
       </c>
-      <c r="AO1" s="22">
+      <c r="AO1" s="20">
         <v>39</v>
       </c>
-      <c r="AP1" s="21">
+      <c r="AP1" s="19">
         <v>40</v>
       </c>
-      <c r="AQ1" s="22">
+      <c r="AQ1" s="20">
         <v>41</v>
       </c>
-      <c r="AR1" s="21">
+      <c r="AR1" s="19">
         <v>42</v>
       </c>
-      <c r="AS1" s="22">
+      <c r="AS1" s="20">
         <v>43</v>
       </c>
-      <c r="AT1" s="21">
+      <c r="AT1" s="19">
         <v>44</v>
       </c>
-      <c r="AU1" s="22">
+      <c r="AU1" s="20">
         <v>45</v>
       </c>
-      <c r="AV1" s="21">
+      <c r="AV1" s="19">
         <v>46</v>
       </c>
-      <c r="AW1" s="22">
+      <c r="AW1" s="20">
         <v>47</v>
       </c>
-      <c r="AX1" s="21">
+      <c r="AX1" s="19">
         <v>48</v>
       </c>
-      <c r="AY1" s="22">
+      <c r="AY1" s="20">
         <v>49</v>
       </c>
-      <c r="AZ1" s="21">
+      <c r="AZ1" s="19">
         <v>50</v>
       </c>
-      <c r="BA1" s="22">
+      <c r="BA1" s="20">
         <v>51</v>
       </c>
-      <c r="BB1" s="21">
+      <c r="BB1" s="19">
         <v>52</v>
       </c>
-      <c r="BC1" s="22">
+      <c r="BC1" s="20">
         <v>53</v>
       </c>
-      <c r="BD1" s="21">
+      <c r="BD1" s="19">
         <v>54</v>
       </c>
-      <c r="BE1" s="22">
+      <c r="BE1" s="20">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1080,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1253,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1426,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1599,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1772,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="47.4" x14ac:dyDescent="0.9">
+    <row r="7" spans="1:62" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1944,11 +1928,11 @@
       <c r="BE7" s="6">
         <v>0</v>
       </c>
-      <c r="BI7" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="BI7" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2127,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2306,7 +2290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2485,7 +2469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2664,7 +2648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2843,7 +2827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3022,7 +3006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3201,7 +3185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3374,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:62" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3547,7 +3531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3720,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3893,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4066,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4239,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4412,7 +4396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4585,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4758,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4931,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5104,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5277,7 +5261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -5450,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -5623,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -5796,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:57" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:57" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -5969,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:57" ht="28.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:57" ht="28.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="4">
         <v>0</v>
       </c>
@@ -6173,20 +6157,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B30CCA-6B6E-4DD0-8945-158CD016E685}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="G1:H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="8" max="8" width="37.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
@@ -6197,7 +6183,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>11</v>
@@ -6205,21 +6191,15 @@
       <c r="F1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17">
         <v>2</v>
       </c>
       <c r="D2">
@@ -6232,14 +6212,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="17">
         <v>8</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <v>2</v>
       </c>
       <c r="D3">
@@ -6252,14 +6232,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>15</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="17">
         <v>2</v>
       </c>
       <c r="D4">
@@ -6272,14 +6252,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="17">
         <v>22</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>2</v>
       </c>
       <c r="D5">
@@ -6292,14 +6272,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>29</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <v>2</v>
       </c>
       <c r="D6">
@@ -6312,14 +6292,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>37</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="17">
         <v>2</v>
       </c>
       <c r="D7">
@@ -6332,14 +6312,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>45</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="17">
         <v>2</v>
       </c>
       <c r="D8">
@@ -6352,14 +6332,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>53</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
         <v>2</v>
       </c>
       <c r="D9">
@@ -6372,14 +6352,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="19">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19">
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="17">
         <v>10</v>
       </c>
       <c r="D10">
@@ -6392,14 +6372,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="17">
         <v>8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>10</v>
       </c>
       <c r="D11">
@@ -6412,14 +6392,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <v>15</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <v>10</v>
       </c>
       <c r="D12">
@@ -6432,14 +6412,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="17">
         <v>22</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="17">
         <v>10</v>
       </c>
       <c r="D13">
@@ -6452,14 +6432,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="17">
         <v>29</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="17">
         <v>10</v>
       </c>
       <c r="D14">
@@ -6472,14 +6452,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="17">
         <v>37</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="17">
         <v>10</v>
       </c>
       <c r="D15">
@@ -6492,14 +6472,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>45</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <v>10</v>
       </c>
       <c r="D16">
@@ -6512,14 +6492,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>53</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <v>10</v>
       </c>
       <c r="D17">
@@ -6532,14 +6512,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="19">
-        <v>1</v>
-      </c>
-      <c r="C18" s="19">
+      <c r="B18" s="17">
+        <v>1</v>
+      </c>
+      <c r="C18" s="17">
         <v>18</v>
       </c>
       <c r="D18">
@@ -6552,14 +6532,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="17">
         <v>8</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="17">
         <v>18</v>
       </c>
       <c r="D19">
@@ -6572,14 +6552,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="17">
         <v>15</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="17">
         <v>18</v>
       </c>
       <c r="D20">
@@ -6592,14 +6572,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <v>22</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="17">
         <v>18</v>
       </c>
       <c r="D21">
@@ -6612,14 +6592,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>29</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="17">
         <v>18</v>
       </c>
       <c r="D22">
@@ -6632,14 +6612,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <v>37</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="17">
         <v>18</v>
       </c>
       <c r="D23">
@@ -6652,14 +6632,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <v>45</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="17">
         <v>18</v>
       </c>
       <c r="D24">
@@ -6672,14 +6652,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>53</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="17">
         <v>18</v>
       </c>
       <c r="D25">
@@ -6692,14 +6672,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="19">
-        <v>1</v>
-      </c>
-      <c r="C26" s="19">
+      <c r="B26" s="17">
+        <v>1</v>
+      </c>
+      <c r="C26" s="17">
         <v>26</v>
       </c>
       <c r="D26">
@@ -6712,14 +6692,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="17">
         <v>8</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="17">
         <v>26</v>
       </c>
       <c r="D27">
@@ -6732,14 +6712,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <v>15</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <v>26</v>
       </c>
       <c r="D28">
@@ -6752,14 +6732,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>28</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="17">
         <v>22</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="17">
         <v>26</v>
       </c>
       <c r="D29">
@@ -6772,14 +6752,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>29</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="17">
         <v>29</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="17">
         <v>26</v>
       </c>
       <c r="D30">
@@ -6792,14 +6772,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>30</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="17">
         <v>37</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="17">
         <v>26</v>
       </c>
       <c r="D31">
@@ -6812,14 +6792,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>31</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="17">
         <v>45</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="17">
         <v>26</v>
       </c>
       <c r="D32">
@@ -6832,14 +6812,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>32</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="17">
         <v>53</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="17">
         <v>26</v>
       </c>
       <c r="D33">
@@ -6852,115 +6832,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>